<commit_message>
Add more tests, minor fixes
</commit_message>
<xml_diff>
--- a/orangecontrib/pumice/datasets/cartoons/cartoons.xlsx
+++ b/orangecontrib/pumice/datasets/cartoons/cartoons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janez/addons/orange3-pumice/orangecontrib/pumice/networks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janez/addons/orange3-pumice/orangecontrib/pumice/datasets/cartoons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536E6624-3008-C040-B770-D53099D42585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8590F6-8D34-C549-9E43-2E3275A78E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18240" yWindow="500" windowWidth="31880" windowHeight="23120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="9900" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="125">
   <si>
     <t>Ana</t>
   </si>
@@ -315,6 +315,99 @@
   </si>
   <si>
     <t>V višave</t>
+  </si>
+  <si>
+    <t>Atlantis The Lost Empire</t>
+  </si>
+  <si>
+    <t>Brave</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Coco</t>
+  </si>
+  <si>
+    <t>Despicable me</t>
+  </si>
+  <si>
+    <t>Encanto</t>
+  </si>
+  <si>
+    <t>Finding Nemo</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>Happy Feet</t>
+  </si>
+  <si>
+    <t>Hotel Transylvania</t>
+  </si>
+  <si>
+    <t>How to Train Your Dragon</t>
+  </si>
+  <si>
+    <t>Ice Age</t>
+  </si>
+  <si>
+    <t>Incredibles</t>
+  </si>
+  <si>
+    <t>Lilo &amp; Stitch</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Megamind</t>
+  </si>
+  <si>
+    <t>Moana</t>
+  </si>
+  <si>
+    <t>Monsters Inc</t>
+  </si>
+  <si>
+    <t>Princess and the Frog</t>
+  </si>
+  <si>
+    <t>Puss in Boots</t>
+  </si>
+  <si>
+    <t>Shrek</t>
+  </si>
+  <si>
+    <t>Spider Man - Into the Spider-Verse</t>
+  </si>
+  <si>
+    <t>Spirited Away</t>
+  </si>
+  <si>
+    <t>Tangled</t>
+  </si>
+  <si>
+    <t>The Boss Baby</t>
+  </si>
+  <si>
+    <t>The Croods</t>
+  </si>
+  <si>
+    <t>The Emperor's New Groove</t>
+  </si>
+  <si>
+    <t>The Lion King</t>
+  </si>
+  <si>
+    <t>Toy Story</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>cartoons-en</t>
   </si>
 </sst>
 </file>
@@ -663,19 +756,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A39"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -683,55 +776,58 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -739,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -786,24 +882,30 @@
       <c r="R2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>18</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -848,18 +950,21 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>94</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -892,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -906,16 +1011,19 @@
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>95</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -936,22 +1044,22 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -960,18 +1068,21 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>96</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -992,10 +1103,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1018,16 +1129,19 @@
       <c r="R7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>97</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1039,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1072,36 +1186,39 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>98</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1116,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1130,19 +1247,22 @@
       <c r="R9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>99</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1151,16 +1271,16 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1186,16 +1306,19 @@
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>100</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1216,13 +1339,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1234,24 +1357,27 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>101</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1278,16 +1404,16 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1298,22 +1424,25 @@
       <c r="R12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>102</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1354,28 +1483,31 @@
       <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14">
-        <v>1</v>
+      <c r="C14" t="s">
+        <v>103</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1384,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1408,18 +1540,21 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>104</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1443,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1455,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1466,16 +1601,19 @@
       <c r="R15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>105</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1496,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1505,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -1522,28 +1660,31 @@
       <c r="R16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>106</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1555,10 +1696,10 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1578,16 +1719,19 @@
       <c r="R17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18">
-        <v>0</v>
+      <c r="C18" t="s">
+        <v>19</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1599,10 +1743,10 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1634,16 +1778,19 @@
       <c r="R18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="C19">
-        <v>0</v>
+      <c r="C19" t="s">
+        <v>107</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1673,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1690,16 +1837,19 @@
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="C20">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>108</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1746,16 +1896,19 @@
       <c r="R20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C21">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>109</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1770,10 +1923,10 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1791,10 +1944,10 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -1802,16 +1955,19 @@
       <c r="R21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="C22">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>110</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1823,10 +1979,10 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1850,39 +2006,42 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>111</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1906,24 +2065,27 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24">
-        <v>0</v>
+      <c r="C24" t="s">
+        <v>112</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1947,39 +2109,42 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
       <c r="R24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>113</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1988,13 +2153,13 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2024,18 +2189,21 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" t="s">
+        <v>20</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2082,16 +2250,19 @@
       <c r="R26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27">
-        <v>0</v>
+      <c r="C27" t="s">
+        <v>21</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2106,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -2118,13 +2289,13 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <v>1</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -2133,21 +2304,24 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" t="s">
+        <v>114</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2165,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2174,36 +2348,39 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>1</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" t="s">
+        <v>115</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2224,10 +2401,10 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2236,30 +2413,33 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29">
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="C30">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>116</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2306,16 +2486,19 @@
       <c r="R30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="C31" t="s">
+        <v>117</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2362,16 +2545,19 @@
       <c r="R31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
       </c>
-      <c r="C32">
-        <v>0</v>
+      <c r="C32" t="s">
+        <v>118</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2395,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -2407,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32">
         <v>0</v>
@@ -2418,16 +2604,19 @@
       <c r="R32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B33" t="s">
         <v>57</v>
       </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="C33" t="s">
+        <v>119</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2448,10 +2637,10 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -2474,16 +2663,19 @@
       <c r="R33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="C34">
-        <v>0</v>
+      <c r="C34" t="s">
+        <v>120</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2530,28 +2722,31 @@
       <c r="R34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="C35">
-        <v>1</v>
+      <c r="C35" t="s">
+        <v>121</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2569,33 +2764,36 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35">
         <v>1</v>
       </c>
       <c r="Q35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C36">
-        <v>0</v>
+      <c r="C36" t="s">
+        <v>122</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2613,45 +2811,48 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>1</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36">
         <v>1</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C37">
-        <v>0</v>
+      <c r="C37" t="s">
+        <v>22</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2698,16 +2899,19 @@
       <c r="R37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B38" t="s">
         <v>62</v>
       </c>
-      <c r="C38">
-        <v>0</v>
+      <c r="C38" t="s">
+        <v>123</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2722,13 +2926,13 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>1</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2743,10 +2947,10 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -2754,16 +2958,19 @@
       <c r="R38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
       </c>
-      <c r="C39">
-        <v>0</v>
+      <c r="C39" t="s">
+        <v>23</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2790,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -2805,9 +3012,12 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39">
         <v>1</v>
       </c>
     </row>

</xml_diff>